<commit_message>
adding profestions choice and langiages to learn
</commit_message>
<xml_diff>
--- a/dataBase/professions.xlsx
+++ b/dataBase/professions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projecs\pythonProject\dataBase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJEKTY\CODING\pythonProject\dataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1865FD0E-8934-4571-A52B-F7B38DF86BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2A6E96-9734-4C43-B01B-B49C57EB19F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25425" yWindow="0" windowWidth="12975" windowHeight="10500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44430" yWindow="3105" windowWidth="28800" windowHeight="15345" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rodzaje Profesji" sheetId="1" r:id="rId1"/>
@@ -790,7 +790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1052,7 +1052,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAF90450-66E3-41E4-99C3-474117DEDDCD}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -1788,8 +1788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E2B6A0-03AF-4B4C-89BF-ABE42E5B5622}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>